<commit_message>
Nova versão do site
</commit_message>
<xml_diff>
--- a/Carteira_Fofo_Projecao_10_Anos.xlsx
+++ b/Carteira_Fofo_Projecao_10_Anos.xlsx
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="51">
   <si>
     <t>Ativo</t>
   </si>
@@ -224,7 +224,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -238,20 +238,42 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -270,6 +292,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDAEEF3"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD8E4BC"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -280,16 +326,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -297,28 +339,31 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="8" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="8" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="8" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="8" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="8" fontId="3" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Moeda" xfId="1" builtinId="4"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -1825,10 +1870,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P14"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1850,551 +1895,554 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="30">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="6" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:16">
-      <c r="A2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="2">
+      <c r="A2" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="12">
         <v>1200</v>
       </c>
-      <c r="D2" s="15">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="E2" s="11">
-        <v>21</v>
-      </c>
-      <c r="F2" s="12">
-        <v>60.76</v>
-      </c>
-      <c r="G2" s="12">
-        <v>1.9</v>
-      </c>
-      <c r="H2" s="13">
-        <v>39.9</v>
-      </c>
-      <c r="I2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" s="17">
-        <v>1501.2</v>
-      </c>
-      <c r="K2" s="17">
-        <v>301.2</v>
-      </c>
-      <c r="L2" s="3"/>
-      <c r="M2" s="18">
-        <v>45470</v>
+      <c r="D2" s="11">
+        <v>9.36</v>
+      </c>
+      <c r="E2" s="13">
+        <v>88</v>
+      </c>
+      <c r="F2" s="14">
+        <v>22.03</v>
+      </c>
+      <c r="G2" s="14">
+        <v>0.42</v>
+      </c>
+      <c r="H2" s="14">
+        <v>36.96</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="15">
+        <v>202.8</v>
+      </c>
+      <c r="K2" s="16">
+        <v>-997.2</v>
+      </c>
+      <c r="L2" s="17"/>
+      <c r="M2" s="10">
+        <v>45835</v>
       </c>
       <c r="N2">
         <f>10*365</f>
         <v>3650</v>
       </c>
-      <c r="P2" s="5"/>
+      <c r="P2" s="2"/>
     </row>
     <row r="3" spans="1:16">
-      <c r="A3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="2">
+      <c r="A3" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="12">
         <v>1200</v>
       </c>
-      <c r="D3" s="15">
-        <v>9.36</v>
-      </c>
-      <c r="E3" s="11">
-        <v>88</v>
-      </c>
-      <c r="F3" s="12">
-        <v>20.420000000000002</v>
-      </c>
-      <c r="G3" s="12">
-        <v>0.42</v>
-      </c>
-      <c r="H3" s="13">
-        <v>36.96</v>
-      </c>
-      <c r="I3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" s="17">
-        <v>202.8</v>
-      </c>
-      <c r="K3" s="17">
-        <v>-997.2</v>
-      </c>
-      <c r="L3" s="3"/>
-      <c r="M3" s="2"/>
-      <c r="P3" s="5"/>
+      <c r="D3" s="11">
+        <v>13.04</v>
+      </c>
+      <c r="E3" s="13">
+        <v>165</v>
+      </c>
+      <c r="F3" s="14">
+        <v>11.13</v>
+      </c>
+      <c r="G3" s="14">
+        <v>0.21</v>
+      </c>
+      <c r="H3" s="14">
+        <v>34.65</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="15">
+        <v>1650.92</v>
+      </c>
+      <c r="K3" s="18">
+        <v>450.92</v>
+      </c>
+      <c r="L3" s="17"/>
+      <c r="M3" s="1"/>
+      <c r="P3" s="2"/>
     </row>
     <row r="4" spans="1:16">
-      <c r="A4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="2">
-        <v>1200</v>
-      </c>
-      <c r="D4" s="15">
-        <v>10.33</v>
-      </c>
-      <c r="E4" s="11">
-        <v>52</v>
-      </c>
-      <c r="F4" s="12">
-        <v>24.19</v>
-      </c>
-      <c r="G4" s="12">
-        <v>0.67</v>
-      </c>
-      <c r="H4" s="13">
-        <v>34.840000000000003</v>
-      </c>
-      <c r="I4" t="s">
-        <v>27</v>
-      </c>
-      <c r="J4" s="4">
-        <v>0</v>
-      </c>
-      <c r="K4" s="17">
-        <v>-1200</v>
-      </c>
-      <c r="L4" s="3"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="14"/>
-      <c r="P4" s="5"/>
+      <c r="A4" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="12">
+        <v>2400</v>
+      </c>
+      <c r="D4" s="11">
+        <v>17.850000000000001</v>
+      </c>
+      <c r="E4" s="13">
+        <v>105</v>
+      </c>
+      <c r="F4" s="14">
+        <v>20.239999999999998</v>
+      </c>
+      <c r="G4" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="H4" s="14">
+        <v>31.5</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" s="15">
+        <v>2409.75</v>
+      </c>
+      <c r="K4" s="18">
+        <v>9.75</v>
+      </c>
+      <c r="L4" s="17"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="8"/>
+      <c r="P4" s="2"/>
     </row>
     <row r="5" spans="1:16">
-      <c r="A5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="2">
+      <c r="A5" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="12">
         <v>1200</v>
       </c>
-      <c r="D5" s="15">
-        <v>13.04</v>
-      </c>
-      <c r="E5" s="11">
-        <v>165</v>
-      </c>
-      <c r="F5" s="12">
-        <v>10.77</v>
-      </c>
-      <c r="G5" s="12">
-        <v>0.21</v>
-      </c>
-      <c r="H5" s="13">
-        <v>34.65</v>
-      </c>
-      <c r="I5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5" s="17">
-        <v>1650.92</v>
-      </c>
-      <c r="K5" s="17">
-        <v>450.92</v>
-      </c>
-      <c r="L5" s="3"/>
-      <c r="M5" s="2"/>
-      <c r="P5" s="5"/>
+      <c r="D5" s="11">
+        <v>10.33</v>
+      </c>
+      <c r="E5" s="13">
+        <v>52</v>
+      </c>
+      <c r="F5" s="14">
+        <v>27.41</v>
+      </c>
+      <c r="G5" s="14">
+        <v>0.67</v>
+      </c>
+      <c r="H5" s="14">
+        <v>34.840000000000003</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="J5" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="K5" s="16">
+        <v>-1200</v>
+      </c>
+      <c r="L5" s="17"/>
+      <c r="M5" s="1"/>
+      <c r="P5" s="2"/>
     </row>
     <row r="6" spans="1:16">
-      <c r="A6" t="s">
+      <c r="A6" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="12">
+        <v>1200</v>
+      </c>
+      <c r="D6" s="11">
+        <v>8.15</v>
+      </c>
+      <c r="E6" s="13">
         <v>31</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="2">
-        <v>2400</v>
-      </c>
-      <c r="D6" s="15">
-        <v>17.850000000000001</v>
-      </c>
-      <c r="E6" s="11">
-        <v>105</v>
-      </c>
-      <c r="F6" s="12">
-        <v>21.99</v>
-      </c>
-      <c r="G6" s="12">
+      <c r="F6" s="14">
+        <v>39.89</v>
+      </c>
+      <c r="G6" s="14">
         <v>0.3</v>
       </c>
-      <c r="H6" s="13">
-        <v>31.5</v>
-      </c>
-      <c r="I6" t="s">
-        <v>32</v>
-      </c>
-      <c r="J6" s="17">
-        <v>2409.75</v>
-      </c>
-      <c r="K6" s="17">
-        <v>9.75</v>
-      </c>
-      <c r="L6" s="3"/>
-      <c r="M6" s="2"/>
-      <c r="P6" s="5"/>
+      <c r="H6" s="14">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="J6" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="K6" s="16">
+        <v>-1200</v>
+      </c>
+      <c r="L6" s="17"/>
+      <c r="M6" s="1"/>
+      <c r="P6" s="2"/>
     </row>
     <row r="7" spans="1:16">
-      <c r="A7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="2">
-        <v>1800</v>
-      </c>
-      <c r="D7" s="15">
-        <v>9.9600000000000009</v>
-      </c>
-      <c r="E7" s="11">
-        <v>24</v>
-      </c>
-      <c r="F7" s="12">
-        <v>101.08</v>
-      </c>
-      <c r="G7" s="12">
-        <v>0.82</v>
-      </c>
-      <c r="H7" s="13">
-        <v>19.68</v>
-      </c>
-      <c r="I7" t="s">
-        <v>34</v>
-      </c>
-      <c r="J7" s="17">
-        <v>207.44</v>
-      </c>
-      <c r="K7" s="17">
-        <v>-1592.56</v>
-      </c>
-      <c r="L7" s="3"/>
-      <c r="M7" s="2"/>
-      <c r="P7" s="5"/>
+      <c r="A7" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="12">
+        <v>2400</v>
+      </c>
+      <c r="D7" s="11">
+        <v>12.76</v>
+      </c>
+      <c r="E7" s="13">
+        <v>11</v>
+      </c>
+      <c r="F7" s="14">
+        <v>105.39</v>
+      </c>
+      <c r="G7" s="14">
+        <v>1</v>
+      </c>
+      <c r="H7" s="14">
+        <v>11</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="J7" s="15">
+        <v>259.5</v>
+      </c>
+      <c r="K7" s="16">
+        <v>-2140.5</v>
+      </c>
+      <c r="L7" s="17"/>
+      <c r="M7" s="1"/>
+      <c r="P7" s="2"/>
     </row>
     <row r="8" spans="1:16">
-      <c r="A8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="A8" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="12">
+        <v>1200</v>
+      </c>
+      <c r="D8" s="11">
+        <v>13.98</v>
+      </c>
+      <c r="E8" s="13">
         <v>14</v>
       </c>
-      <c r="C8" s="2">
-        <v>1200</v>
-      </c>
-      <c r="D8" s="15">
-        <v>8.65</v>
-      </c>
-      <c r="E8" s="11">
-        <v>34</v>
-      </c>
-      <c r="F8" s="12">
-        <v>36.39</v>
-      </c>
-      <c r="G8" s="12">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="H8" s="13">
-        <v>18.7</v>
-      </c>
-      <c r="I8" t="s">
-        <v>36</v>
-      </c>
-      <c r="J8" s="17">
-        <v>342.8</v>
-      </c>
-      <c r="K8" s="17">
-        <v>-857.2</v>
-      </c>
-      <c r="L8" s="3"/>
-      <c r="M8" s="2"/>
-      <c r="P8" s="5"/>
+      <c r="F8" s="14">
+        <v>82.33</v>
+      </c>
+      <c r="G8" s="14">
+        <v>1.05</v>
+      </c>
+      <c r="H8" s="14">
+        <v>14.7</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="J8" s="15">
+        <v>1273.93</v>
+      </c>
+      <c r="K8" s="18">
+        <v>73.930000000000007</v>
+      </c>
+      <c r="L8" s="17"/>
+      <c r="M8" s="1"/>
+      <c r="P8" s="2"/>
     </row>
     <row r="9" spans="1:16">
-      <c r="A9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="2">
+      <c r="A9" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="12">
         <v>1200</v>
       </c>
-      <c r="D9" s="15">
-        <v>13.98</v>
-      </c>
-      <c r="E9" s="11">
-        <v>14</v>
-      </c>
-      <c r="F9" s="12">
-        <v>79.709999999999994</v>
-      </c>
-      <c r="G9" s="12">
-        <v>1.05</v>
-      </c>
-      <c r="H9" s="13">
-        <v>14.7</v>
-      </c>
-      <c r="I9" t="s">
+      <c r="D9" s="11">
+        <v>16.649999999999999</v>
+      </c>
+      <c r="E9" s="13">
         <v>38</v>
       </c>
-      <c r="J9" s="17">
-        <v>1193.25</v>
-      </c>
-      <c r="K9" s="17">
-        <v>-6.75</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="M9" s="2"/>
-      <c r="P9" s="5"/>
+      <c r="F9" s="14">
+        <v>32.51</v>
+      </c>
+      <c r="G9" s="14">
+        <v>0.34</v>
+      </c>
+      <c r="H9" s="14">
+        <v>12.76</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="J9" s="15">
+        <v>1223.6199999999999</v>
+      </c>
+      <c r="K9" s="18">
+        <v>23.62</v>
+      </c>
+      <c r="L9" s="17"/>
+      <c r="M9" s="1"/>
+      <c r="P9" s="2"/>
     </row>
     <row r="10" spans="1:16">
-      <c r="A10" t="s">
+      <c r="A10" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="12">
         <v>1200</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="11">
         <v>13.52</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E10" s="13">
         <v>13</v>
       </c>
-      <c r="F10" s="12">
-        <v>92.03</v>
-      </c>
-      <c r="G10" s="12">
+      <c r="F10" s="14">
+        <v>94.85</v>
+      </c>
+      <c r="G10" s="14">
         <v>1</v>
       </c>
-      <c r="H10" s="13">
+      <c r="H10" s="14">
         <v>13</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="J10" s="17">
+      <c r="J10" s="15">
         <v>924.6</v>
       </c>
-      <c r="K10" s="17">
+      <c r="K10" s="16">
         <v>-275.39999999999998</v>
       </c>
-      <c r="L10" s="3"/>
-      <c r="M10" s="2"/>
-      <c r="P10" s="5"/>
+      <c r="L10" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="M10" s="1"/>
+      <c r="P10" s="2"/>
     </row>
     <row r="11" spans="1:16">
-      <c r="A11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="2">
+      <c r="A11" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="12">
         <v>1200</v>
       </c>
-      <c r="D11" s="15">
-        <v>16.649999999999999</v>
-      </c>
-      <c r="E11" s="11">
-        <v>38</v>
-      </c>
-      <c r="F11" s="12">
-        <v>29.72</v>
-      </c>
-      <c r="G11" s="12">
-        <v>0.34</v>
-      </c>
-      <c r="H11" s="13">
-        <v>12.76</v>
-      </c>
-      <c r="I11" t="s">
-        <v>42</v>
-      </c>
-      <c r="J11" s="17">
-        <v>1223.6199999999999</v>
-      </c>
-      <c r="K11" s="17">
-        <v>23.62</v>
-      </c>
-      <c r="L11" s="3"/>
-      <c r="M11" s="2"/>
-      <c r="P11" s="5"/>
+      <c r="D11" s="11">
+        <v>8.65</v>
+      </c>
+      <c r="E11" s="13">
+        <v>34</v>
+      </c>
+      <c r="F11" s="14">
+        <v>42.86</v>
+      </c>
+      <c r="G11" s="14">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H11" s="14">
+        <v>18.7</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="J11" s="15">
+        <v>342.8</v>
+      </c>
+      <c r="K11" s="16">
+        <v>-857.2</v>
+      </c>
+      <c r="L11" s="17"/>
+      <c r="M11" s="1"/>
+      <c r="P11" s="2"/>
     </row>
     <row r="12" spans="1:16">
-      <c r="A12" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="2">
-        <v>2400</v>
-      </c>
-      <c r="D12" s="15">
-        <v>12.76</v>
-      </c>
-      <c r="E12" s="11">
-        <v>11</v>
-      </c>
-      <c r="F12" s="12">
-        <v>104.78</v>
-      </c>
-      <c r="G12" s="12">
-        <v>1</v>
-      </c>
-      <c r="H12" s="13">
-        <v>11</v>
-      </c>
-      <c r="I12" t="s">
-        <v>44</v>
-      </c>
-      <c r="J12" s="17">
-        <v>259.5</v>
-      </c>
-      <c r="K12" s="17">
-        <v>-2140.5</v>
-      </c>
-      <c r="L12" s="3"/>
-      <c r="M12" s="2"/>
-      <c r="P12" s="5"/>
+      <c r="A12" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="12">
+        <v>1200</v>
+      </c>
+      <c r="D12" s="11">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="E12" s="13">
+        <v>21</v>
+      </c>
+      <c r="F12" s="14">
+        <v>65.36</v>
+      </c>
+      <c r="G12" s="14">
+        <v>1.9</v>
+      </c>
+      <c r="H12" s="14">
+        <v>39.9</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="J12" s="15">
+        <v>1501.2</v>
+      </c>
+      <c r="K12" s="18">
+        <v>301.2</v>
+      </c>
+      <c r="L12" s="17"/>
+      <c r="M12" s="1"/>
+      <c r="P12" s="2"/>
     </row>
     <row r="13" spans="1:16">
-      <c r="A13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="2">
-        <v>1200</v>
-      </c>
-      <c r="D13" s="15">
-        <v>8.15</v>
-      </c>
-      <c r="E13" s="11">
-        <v>31</v>
-      </c>
-      <c r="F13" s="12">
-        <v>37.99</v>
-      </c>
-      <c r="G13" s="12">
-        <v>0.3</v>
-      </c>
-      <c r="H13" s="13">
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="I13" t="s">
-        <v>46</v>
-      </c>
-      <c r="J13" s="4" t="s">
+      <c r="A13" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="12">
+        <v>1800</v>
+      </c>
+      <c r="D13" s="11">
+        <v>9.2899999999999991</v>
+      </c>
+      <c r="E13" s="13">
+        <v>11</v>
+      </c>
+      <c r="F13" s="14">
+        <v>109.02</v>
+      </c>
+      <c r="G13" s="14">
+        <v>0.81</v>
+      </c>
+      <c r="H13" s="14">
+        <v>8.91</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="J13" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="K13" s="17">
-        <v>-1200</v>
-      </c>
-      <c r="L13" s="3"/>
-      <c r="M13" s="2"/>
-      <c r="P13" s="5"/>
+      <c r="K13" s="16">
+        <v>-1800</v>
+      </c>
+      <c r="L13" s="17"/>
+      <c r="M13" s="1"/>
+      <c r="P13" s="2"/>
     </row>
     <row r="14" spans="1:16">
-      <c r="A14" t="s">
-        <v>47</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="2">
+      <c r="A14" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="12">
         <v>1800</v>
       </c>
-      <c r="D14" s="15">
-        <v>9.2899999999999991</v>
-      </c>
-      <c r="E14" s="11">
-        <v>11</v>
-      </c>
-      <c r="F14" s="12">
-        <v>107.95</v>
-      </c>
-      <c r="G14" s="12">
-        <v>0.81</v>
-      </c>
-      <c r="H14" s="13">
-        <v>8.91</v>
-      </c>
-      <c r="I14" t="s">
-        <v>48</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="K14" s="17">
-        <v>-1800</v>
-      </c>
-      <c r="L14" s="3"/>
-      <c r="M14" s="2"/>
-      <c r="P14" s="5"/>
+      <c r="D14" s="11">
+        <v>9.9600000000000009</v>
+      </c>
+      <c r="E14" s="13">
+        <v>24</v>
+      </c>
+      <c r="F14" s="14">
+        <v>103.75</v>
+      </c>
+      <c r="G14" s="14">
+        <v>0.82</v>
+      </c>
+      <c r="H14" s="14">
+        <v>19.68</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="J14" s="15">
+        <v>207.44</v>
+      </c>
+      <c r="K14" s="16">
+        <v>-1592.56</v>
+      </c>
+      <c r="L14" s="17"/>
+      <c r="M14" s="1"/>
+      <c r="P14" s="2"/>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="J15" s="19"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:L14">
@@ -2402,15 +2450,8 @@
       <sortCondition descending="1" ref="H1:H14"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="K2:K14">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>